<commit_message>
Started removing slice concept.
</commit_message>
<xml_diff>
--- a/.Docs/Stories.xlsx
+++ b/.Docs/Stories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>Story</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>bring lowest ingredient % to 0</t>
+  </si>
+  <si>
+    <t>an ingredient % is changed to 100%</t>
+  </si>
+  <si>
+    <t>all other ingredients should be 0</t>
+  </si>
+  <si>
+    <t>100% change</t>
+  </si>
+  <si>
+    <t>&lt; 0 change</t>
+  </si>
+  <si>
+    <t>&gt; 100 change</t>
+  </si>
+  <si>
+    <t>an ingredient % is changed to a negative value</t>
+  </si>
+  <si>
+    <t>change will be interpreted as 0</t>
+  </si>
+  <si>
+    <t>an ingredient % is changed to a value &gt; 100</t>
+  </si>
+  <si>
+    <t>change will be interpreted as 100</t>
   </si>
 </sst>
 </file>
@@ -193,15 +220,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +547,7 @@
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
@@ -542,7 +570,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -558,7 +586,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -572,85 +604,79 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="1" t="s">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>50</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>50</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f>SUM(G9:J9)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>SUM(G10:J10)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>21</v>
-      </c>
-      <c r="I10">
-        <v>20</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <v>40</v>
-      </c>
-      <c r="H11">
-        <v>40</v>
       </c>
       <c r="I11">
         <v>20</v>
@@ -658,389 +684,501 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="L11">
-        <f>SUM(G11:J11)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>40</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>SUM(G12:J12)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>19</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>40</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>40</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>20</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f>SUM(G13:J13)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>SUM(G14:J14)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>21</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15">
-        <v>39</v>
-      </c>
-      <c r="H15">
-        <v>39</v>
-      </c>
-      <c r="I15">
-        <v>18</v>
       </c>
       <c r="J15">
         <v>4</v>
       </c>
-      <c r="L15">
-        <f>SUM(G15:J15)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17">
-        <f>SUM(G17:J17)</f>
-        <v>0</v>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>39</v>
+      </c>
+      <c r="H16">
+        <v>39</v>
+      </c>
+      <c r="I16">
+        <v>18</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <f>SUM(G16:J16)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="L18">
+        <f>SUM(G18:J18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>35</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>20</v>
       </c>
-      <c r="L19">
-        <f>SUM(G19:J19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
+      <c r="L20">
+        <f>SUM(G20:J20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G22" s="3">
         <v>59</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H22" s="3">
         <v>40</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I22" s="3">
         <v>1</v>
       </c>
-      <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4">
-        <f>SUM(G21:J21)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3">
+        <f>SUM(G22:J22)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
         <v>2</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G24" s="3">
         <v>59</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H24" s="3">
         <v>38</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I24" s="3">
         <v>1</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J24" s="3">
         <v>2</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4">
-        <f>SUM(G23:J23)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3">
+        <f>SUM(G24:J24)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="5" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G28" s="3">
         <v>59</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H28" s="3">
         <v>40</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I28" s="3">
         <v>1</v>
       </c>
-      <c r="J27" s="4">
-        <v>0</v>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4">
-        <f>SUM(G27:J27)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4" t="s">
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3">
+        <f>SUM(G28:J28)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3">
         <v>2</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4" t="s">
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G30" s="3">
         <v>59</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H30" s="3">
         <v>39</v>
       </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="4">
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
         <v>2</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4">
-        <f>SUM(G29:J29)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="L30" s="3">
+        <f>SUM(G30:J30)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>14</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>17</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>19</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>40</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>40</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>20</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <f>SUM(G31:J31)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>SUM(G32:J32)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>24</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>21</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33">
-        <v>40</v>
-      </c>
-      <c r="H33">
-        <v>40</v>
-      </c>
-      <c r="I33">
-        <v>19</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
-      <c r="L33">
-        <f>SUM(G33:J33)</f>
-        <v>100</v>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <v>40</v>
+      </c>
+      <c r="I34">
+        <v>19</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <f>SUM(G34:J34)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36">
+        <v>40</v>
+      </c>
+      <c r="H36">
+        <v>40</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>SUM(G36:J36)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f>SUM(G38:J38)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the concept of filler to the pie and wired announcing filler changes when other ingredients are changed.  Separated editable ingredients from non-editable (e.g. filler).
</commit_message>
<xml_diff>
--- a/.Docs/Stories.xlsx
+++ b/.Docs/Stories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>Story</t>
   </si>
@@ -163,6 +163,39 @@
   </si>
   <si>
     <t>change will be interpreted as 100</t>
+  </si>
+  <si>
+    <t>Filler</t>
+  </si>
+  <si>
+    <t>Proposed</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>&lt; Filler</t>
+  </si>
+  <si>
+    <t>&gt; Filler</t>
+  </si>
+  <si>
+    <t>= Filler</t>
+  </si>
+  <si>
+    <t>No Filler</t>
+  </si>
+  <si>
+    <t>And pie has filler</t>
+  </si>
+  <si>
+    <t>And pie has NO filler</t>
+  </si>
+  <si>
+    <t>an ingrediuient % is changed</t>
+  </si>
+  <si>
+    <t>should reject the proposal</t>
   </si>
 </sst>
 </file>
@@ -220,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -230,6 +263,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1213,157 @@
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46">
+        <v>40</v>
+      </c>
+      <c r="H46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51">
+        <v>40</v>
+      </c>
+      <c r="H51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>51</v>
+      </c>
+      <c r="H53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" t="s">
+        <v>49</v>
+      </c>
+      <c r="H55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56">
+        <v>40</v>
+      </c>
+      <c r="H56">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>51</v>
+      </c>
+      <c r="H58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
balanced the pie with filler...finally!
</commit_message>
<xml_diff>
--- a/.Docs/Stories.xlsx
+++ b/.Docs/Stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
   <si>
     <t>Story</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>should reject the proposal</t>
+  </si>
+  <si>
+    <t>Proposal</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -264,6 +267,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
@@ -1374,12 +1380,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <f>SUM(C4:E4)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>SUM(C6:E6)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <f>SUM(C8:E8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <f>40/90</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>50</v>
+      </c>
+      <c r="M18">
+        <f>50/90</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>